<commit_message>
add flexible reaction volumes in 02-ont protocol
</commit_message>
<xml_diff>
--- a/templates/02-ont-gDNA.xlsx
+++ b/templates/02-ont-gDNA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/Desktop/2210-alarawi-ont/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D19E8-3680-BB48-BE06-61C40D2B2263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7236A84B-5572-FA48-B7B8-1FC3E61CA409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="1360" windowWidth="27920" windowHeight="15940" xr2:uid="{0E74BB9A-F8B8-AA47-B7C7-EA2C2417D685}"/>
   </bookViews>
@@ -1111,7 +1111,7 @@
     <t>sample 17</t>
   </si>
   <si>
-    <t>Used here - 100 ng @ 7 Mb genome = 0.023 fmoles</t>
+    <t>Used here - 100 ng @ 30 kb DNA genome = 5.4 fmoles</t>
   </si>
 </sst>
 </file>
@@ -1275,13 +1275,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1333,14 +1333,14 @@
     <tableColumn id="4" xr3:uid="{80D148B5-CECA-CA44-B1DD-F9E1A8DAA6A0}" name="fmol/ul" dataDxfId="4">
       <calculatedColumnFormula>F9/((E9*617.96)+36.04) * 1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6A4DD60B-B1AB-FF44-9E4F-4697D7C0CC9E}" name="ul plasmid" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{6A4DD60B-B1AB-FF44-9E4F-4697D7C0CC9E}" name="ul plasmid" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{53D08A06-9EBD-1143-A0BC-3E9BC0C89175}" name="ul water to 4.5" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{53D08A06-9EBD-1143-A0BC-3E9BC0C89175}" name="ul water to 4.5" dataDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0EE7AD1A-A1CC-364C-B346-C43B6AB6BFEF}" name="dest well" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{DDAE90F6-C57C-A64E-B7AF-286C3EB0FE38}" name="barcode well" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{0EE7AD1A-A1CC-364C-B346-C43B6AB6BFEF}" name="dest well" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{DDAE90F6-C57C-A64E-B7AF-286C3EB0FE38}" name="barcode well" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1657,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842AFD07-9B34-384A-83A8-BAD898DE59C4}">
-  <dimension ref="B1:R105"/>
+  <dimension ref="B1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1680,22 +1680,22 @@
     <col min="16" max="16" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>319</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1714,10 +1714,10 @@
         <v>9</v>
       </c>
       <c r="J5">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M7" t="s">
         <v>323</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>306</v>
       </c>
@@ -1794,11 +1794,11 @@
       <c r="P8" t="s">
         <v>313</v>
       </c>
-      <c r="R8" t="s">
+      <c r="Q8" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>113</v>
       </c>
@@ -1809,22 +1809,22 @@
         <v>210</v>
       </c>
       <c r="E9">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F9">
         <v>14</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" ref="G9:G23" si="0">F9/((E9*617.96)+36.04) * 1000000</f>
-        <v>4.5310375547612811E-3</v>
+        <v>0.75517146652536016</v>
       </c>
       <c r="H9" s="2" cm="1">
         <f t="array" ref="H9">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>8.8280001029714281</v>
+        <v>7.1506939011428576</v>
       </c>
       <c r="I9" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>0.17199989702857188</v>
+        <v>1.8493060988571424</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>113</v>
@@ -1840,7 +1840,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>114</v>
       </c>
@@ -1851,22 +1851,22 @@
         <v>211</v>
       </c>
       <c r="E10">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F10">
         <v>81</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>2.6215288709690268E-2</v>
+        <v>4.3692063420395835</v>
       </c>
       <c r="H10" s="2" cm="1">
         <f t="array" ref="H10">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.5258271782913582</v>
+        <v>1.2359224026666669</v>
       </c>
       <c r="I10" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>7.4741728217086418</v>
+        <v>7.7640775973333334</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>114</v>
@@ -1882,7 +1882,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>115</v>
       </c>
@@ -1893,22 +1893,22 @@
         <v>212</v>
       </c>
       <c r="E11">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F11">
         <v>40</v>
       </c>
       <c r="G11" s="2">
         <f>F11/((E11*617.96)+36.04) * 1000000</f>
-        <v>1.2945821585032231E-2</v>
+        <v>2.1576327615010289</v>
       </c>
       <c r="H11" s="2" cm="1">
         <f t="array" ref="H11">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>3.0898000360400002</v>
+        <v>2.5027428654000001</v>
       </c>
       <c r="I11" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>5.9101999639600002</v>
+        <v>6.4972571345999999</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>115</v>
@@ -1918,7 +1918,7 @@
         <v>C01</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>116</v>
       </c>
@@ -1929,22 +1929,22 @@
         <v>213</v>
       </c>
       <c r="E12">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F12">
         <v>22</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>7.1202018717677279E-3</v>
+        <v>1.186698018825566</v>
       </c>
       <c r="H12" s="2" cm="1">
         <f t="array" ref="H12">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>5.6178182473454541</v>
+        <v>4.5504415734545454</v>
       </c>
       <c r="I12" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>3.3821817526545459</v>
+        <v>4.4495584265454546</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>116</v>
@@ -1960,7 +1960,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>117</v>
       </c>
@@ -1971,14 +1971,14 @@
         <v>214</v>
       </c>
       <c r="E13">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F13">
         <v>344</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>0.11133406563127719</v>
+        <v>18.555641748908851</v>
       </c>
       <c r="H13" s="2" cm="1">
         <f t="array" ref="H13">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
@@ -2000,7 +2000,7 @@
       </c>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>118</v>
       </c>
@@ -2011,22 +2011,22 @@
         <v>215</v>
       </c>
       <c r="E14">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F14">
         <v>216</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>6.9907436559174058E-2</v>
+        <v>11.651216912105557</v>
       </c>
       <c r="H14" s="2" cm="1">
         <f t="array" ref="H14">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0.5721851918592592</v>
+        <v>0.5</v>
       </c>
       <c r="I14" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>8.4278148081407416</v>
+        <v>8.5</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>118</v>
@@ -2036,7 +2036,7 @@
         <v>F01</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>119</v>
       </c>
@@ -2047,22 +2047,22 @@
         <v>216</v>
       </c>
       <c r="E15">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F15">
         <v>62</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>2.0066023456799958E-2</v>
+        <v>3.3443307803265947</v>
       </c>
       <c r="H15" s="2" cm="1">
         <f t="array" ref="H15">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.9934193780903229</v>
+        <v>1.6146728163870969</v>
       </c>
       <c r="I15" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>7.0065806219096771</v>
+        <v>7.3853271836129029</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>119</v>
@@ -2072,7 +2072,7 @@
         <v>G01</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>120</v>
       </c>
@@ -2083,22 +2083,22 @@
         <v>217</v>
       </c>
       <c r="E16">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F16">
         <v>75</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>2.4273415471935435E-2</v>
+        <v>4.0455614278144294</v>
       </c>
       <c r="H16" s="2" cm="1">
         <f t="array" ref="H16">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.6478933525546666</v>
+        <v>1.33479619488</v>
       </c>
       <c r="I16" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>7.3521066474453338</v>
+        <v>7.66520380512</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>120</v>
@@ -2119,22 +2119,22 @@
         <v>218</v>
       </c>
       <c r="E17">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F17">
         <v>82</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v>2.6538934249316078E-2</v>
+        <v>4.4231471610771091</v>
       </c>
       <c r="H17" s="2" cm="1">
         <f t="array" ref="H17">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.5072195297756097</v>
+        <v>1.2208501782439025</v>
       </c>
       <c r="I17" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>7.4927804702243908</v>
+        <v>7.7791498217560973</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>121</v>
@@ -2155,22 +2155,22 @@
         <v>219</v>
       </c>
       <c r="E18">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F18">
         <v>40</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>1.2945821585032231E-2</v>
+        <v>2.1576327615010289</v>
       </c>
       <c r="H18" s="2" cm="1">
         <f t="array" ref="H18">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>3.0898000360400002</v>
+        <v>2.5027428654000001</v>
       </c>
       <c r="I18" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>5.9101999639600002</v>
+        <v>6.4972571345999999</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>122</v>
@@ -2191,22 +2191,22 @@
         <v>220</v>
       </c>
       <c r="E19">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F19">
         <v>121</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>3.9161110294722502E-2</v>
+        <v>6.5268391035406133</v>
       </c>
       <c r="H19" s="2" cm="1">
         <f t="array" ref="H19">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.0214214995173554</v>
+        <v>0.82735301335537192</v>
       </c>
       <c r="I19" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>7.9785785004826444</v>
+        <v>8.1726469866446276</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>123</v>
@@ -2227,22 +2227,22 @@
         <v>221</v>
       </c>
       <c r="E20">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F20">
         <v>141</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="0"/>
-        <v>4.5634021087238616E-2</v>
+        <v>7.6056554842911277</v>
       </c>
       <c r="H20" s="2" cm="1">
         <f t="array" ref="H20">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0.87653901731631212</v>
+        <v>0.70999797600000003</v>
       </c>
       <c r="I20" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>8.1234609826836888</v>
+        <v>8.2900020239999996</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>124</v>
@@ -2263,22 +2263,22 @@
         <v>222</v>
       </c>
       <c r="E21">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F21">
         <v>194</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
-        <v>6.2787234687406324E-2</v>
+        <v>10.46451889327999</v>
       </c>
       <c r="H21" s="2" cm="1">
         <f t="array" ref="H21">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0.63707217237938152</v>
+        <v>0.5160294567835052</v>
       </c>
       <c r="I21" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>8.3629278276206183</v>
+        <v>8.4839705432164951</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>125</v>
@@ -2299,22 +2299,22 @@
         <v>223</v>
       </c>
       <c r="E22">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F22">
         <v>224</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v>7.2496600876180498E-2</v>
+        <v>12.082743464405763</v>
       </c>
       <c r="H22" s="2" cm="1">
         <f t="array" ref="H22">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0.55175000643571426</v>
+        <v>0.5</v>
       </c>
       <c r="I22" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>8.4482499935642856</v>
+        <v>8.5</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>126</v>
@@ -2335,22 +2335,22 @@
         <v>224</v>
       </c>
       <c r="E23">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F23">
         <v>102</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>3.3011845041832188E-2</v>
+        <v>5.5019635418276236</v>
       </c>
       <c r="H23" s="2" cm="1">
         <f t="array" ref="H23">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>1.2116862886431374</v>
+        <v>0.98146779035294129</v>
       </c>
       <c r="I23" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>7.7883137113568628</v>
+        <v>8.0185322096470593</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>127</v>
@@ -2371,22 +2371,22 @@
         <v>225</v>
       </c>
       <c r="E24">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F24">
         <v>130</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" ref="G24" si="1">F24/((E24*617.96)+36.04) * 1000000</f>
-        <v>4.2073920151354756E-2</v>
+        <v>7.0123064748783444</v>
       </c>
       <c r="H24" s="2" cm="1">
         <f t="array" ref="H24">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0.95070770339692301</v>
+        <v>0.77007472781538466</v>
       </c>
       <c r="I24" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>8.0492922966030775</v>
+        <v>8.2299252721846159</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>128</v>
@@ -2407,22 +2407,22 @@
         <v>226</v>
       </c>
       <c r="E25">
-        <v>5000000</v>
+        <v>30000</v>
       </c>
       <c r="F25">
         <v>167</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" ref="G25:G38" si="2">F25/((E25*617.96)+36.04) * 1000000</f>
-        <v>5.4048805117509563E-2</v>
+        <v>9.0081167792667962</v>
       </c>
       <c r="H25" s="2" cm="1">
         <f t="array" ref="H25">_xlfn.IFS(Table1[[#This Row],[fmol/ul]]=0,0,$J$5/Table1[[#This Row],[fmol/ul]]&lt;0.5,0.5,$J$5/Table1[[#This Row],[fmol/ul]]&gt;9,9,  TRUE, $J$5/Table1[[#This Row],[fmol/ul]])</f>
-        <v>0.74007186491976051</v>
+        <v>0.59945936895808383</v>
       </c>
       <c r="I25" s="2">
         <f>IF(Table1[[#This Row],[ul plasmid]]=0,0,9-Table1[[#This Row],[ul plasmid]])</f>
-        <v>8.2599281350802389</v>
+        <v>8.4005406310419168</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>129</v>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="C2" s="9">
         <f>main!H9</f>
-        <v>8.8280001029714281</v>
+        <v>7.1506939011428576</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>IF(C2=0, "", "A01")</f>
@@ -5660,7 +5660,7 @@
       </c>
       <c r="F2" s="9">
         <f>main!I9</f>
-        <v>0.17199989702857188</v>
+        <v>1.8493060988571424</v>
       </c>
       <c r="G2" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D9,Table2[name],Table2[well],"")</f>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="C3" s="9">
         <f>main!H10</f>
-        <v>1.5258271782913582</v>
+        <v>1.2359224026666669</v>
       </c>
       <c r="D3" s="8" t="str">
         <f t="shared" ref="D3:D66" si="0">IF(C3=0, "", "A01")</f>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="F3" s="9">
         <f>main!I10</f>
-        <v>7.4741728217086418</v>
+        <v>7.7640775973333334</v>
       </c>
       <c r="G3" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D10,Table2[name],Table2[well],"")</f>
@@ -5719,7 +5719,7 @@
       </c>
       <c r="C4" s="9">
         <f>main!H11</f>
-        <v>3.0898000360400002</v>
+        <v>2.5027428654000001</v>
       </c>
       <c r="D4" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5730,7 +5730,7 @@
       </c>
       <c r="F4" s="9">
         <f>main!I11</f>
-        <v>5.9101999639600002</v>
+        <v>6.4972571345999999</v>
       </c>
       <c r="G4" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D11,Table2[name],Table2[well],"")</f>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="C5" s="9">
         <f>main!H12</f>
-        <v>5.6178182473454541</v>
+        <v>4.5504415734545454</v>
       </c>
       <c r="D5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5765,7 +5765,7 @@
       </c>
       <c r="F5" s="9">
         <f>main!I12</f>
-        <v>3.3821817526545459</v>
+        <v>4.4495584265454546</v>
       </c>
       <c r="G5" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D12,Table2[name],Table2[well],"")</f>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="C7" s="9">
         <f>main!H14</f>
-        <v>0.5721851918592592</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="F7" s="9">
         <f>main!I14</f>
-        <v>8.4278148081407416</v>
+        <v>8.5</v>
       </c>
       <c r="G7" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D14,Table2[name],Table2[well],"")</f>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="C8" s="9">
         <f>main!H15</f>
-        <v>1.9934193780903229</v>
+        <v>1.6146728163870969</v>
       </c>
       <c r="D8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5870,7 +5870,7 @@
       </c>
       <c r="F8" s="9">
         <f>main!I15</f>
-        <v>7.0065806219096771</v>
+        <v>7.3853271836129029</v>
       </c>
       <c r="G8" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D15,Table2[name],Table2[well],"")</f>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="C9" s="9">
         <f>main!H16</f>
-        <v>1.6478933525546666</v>
+        <v>1.33479619488</v>
       </c>
       <c r="D9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="F9" s="9">
         <f>main!I16</f>
-        <v>7.3521066474453338</v>
+        <v>7.66520380512</v>
       </c>
       <c r="G9" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D16,Table2[name],Table2[well],"")</f>
@@ -5929,7 +5929,7 @@
       </c>
       <c r="C10" s="9">
         <f>main!H17</f>
-        <v>1.5072195297756097</v>
+        <v>1.2208501782439025</v>
       </c>
       <c r="D10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5940,7 +5940,7 @@
       </c>
       <c r="F10" s="9">
         <f>main!I17</f>
-        <v>7.4927804702243908</v>
+        <v>7.7791498217560973</v>
       </c>
       <c r="G10" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D17,Table2[name],Table2[well],"")</f>
@@ -5964,7 +5964,7 @@
       </c>
       <c r="C11" s="9">
         <f>main!H18</f>
-        <v>3.0898000360400002</v>
+        <v>2.5027428654000001</v>
       </c>
       <c r="D11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5975,7 +5975,7 @@
       </c>
       <c r="F11" s="9">
         <f>main!I18</f>
-        <v>5.9101999639600002</v>
+        <v>6.4972571345999999</v>
       </c>
       <c r="G11" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D18,Table2[name],Table2[well],"")</f>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="C12" s="9">
         <f>main!H19</f>
-        <v>1.0214214995173554</v>
+        <v>0.82735301335537192</v>
       </c>
       <c r="D12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="F12" s="9">
         <f>main!I19</f>
-        <v>7.9785785004826444</v>
+        <v>8.1726469866446276</v>
       </c>
       <c r="G12" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D19,Table2[name],Table2[well],"")</f>
@@ -6034,7 +6034,7 @@
       </c>
       <c r="C13" s="9">
         <f>main!H20</f>
-        <v>0.87653901731631212</v>
+        <v>0.70999797600000003</v>
       </c>
       <c r="D13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="F13" s="9">
         <f>main!I20</f>
-        <v>8.1234609826836888</v>
+        <v>8.2900020239999996</v>
       </c>
       <c r="G13" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D20,Table2[name],Table2[well],"")</f>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="C14" s="9">
         <f>main!H21</f>
-        <v>0.63707217237938152</v>
+        <v>0.5160294567835052</v>
       </c>
       <c r="D14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6080,7 +6080,7 @@
       </c>
       <c r="F14" s="9">
         <f>main!I21</f>
-        <v>8.3629278276206183</v>
+        <v>8.4839705432164951</v>
       </c>
       <c r="G14" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D21,Table2[name],Table2[well],"")</f>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="C15" s="9">
         <f>main!H22</f>
-        <v>0.55175000643571426</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6115,7 +6115,7 @@
       </c>
       <c r="F15" s="9">
         <f>main!I22</f>
-        <v>8.4482499935642856</v>
+        <v>8.5</v>
       </c>
       <c r="G15" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D22,Table2[name],Table2[well],"")</f>
@@ -6139,7 +6139,7 @@
       </c>
       <c r="C16" s="9">
         <f>main!H23</f>
-        <v>1.2116862886431374</v>
+        <v>0.98146779035294129</v>
       </c>
       <c r="D16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6150,7 +6150,7 @@
       </c>
       <c r="F16" s="9">
         <f>main!I23</f>
-        <v>7.7883137113568628</v>
+        <v>8.0185322096470593</v>
       </c>
       <c r="G16" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D23,Table2[name],Table2[well],"")</f>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="C17" s="9">
         <f>main!H24</f>
-        <v>0.95070770339692301</v>
+        <v>0.77007472781538466</v>
       </c>
       <c r="D17" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="F17" s="9">
         <f>main!I24</f>
-        <v>8.0492922966030775</v>
+        <v>8.2299252721846159</v>
       </c>
       <c r="G17" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D24,Table2[name],Table2[well],"")</f>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="C18" s="9">
         <f>main!H25</f>
-        <v>0.74007186491976051</v>
+        <v>0.59945936895808383</v>
       </c>
       <c r="D18" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6220,7 +6220,7 @@
       </c>
       <c r="F18" s="9">
         <f>main!I25</f>
-        <v>8.2599281350802389</v>
+        <v>8.4005406310419168</v>
       </c>
       <c r="G18" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D25,Table2[name],Table2[well],"")</f>

</xml_diff>

<commit_message>
added blinking in sanger protocol
</commit_message>
<xml_diff>
--- a/templates/02-ont-gDNA.xlsx
+++ b/templates/02-ont-gDNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloas/code/opentrons/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D422C64-C8BD-7F4C-8F01-38CDDFF74956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD406013-3B11-4743-967A-D09CBEC6D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2600" yWindow="-20500" windowWidth="27920" windowHeight="15940" xr2:uid="{0E74BB9A-F8B8-AA47-B7C7-EA2C2417D685}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{0E74BB9A-F8B8-AA47-B7C7-EA2C2417D685}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="340">
   <si>
     <t>The incubations are done off instrument</t>
   </si>
@@ -1239,7 +1239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1270,7 +1270,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1289,17 +1288,13 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -1317,16 +1312,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1370,19 +1369,19 @@
     <tableColumn id="8" xr3:uid="{FA78698F-F611-D543-B141-D777144BECEE}" name="source well" dataDxfId="6"/>
     <tableColumn id="1" xr3:uid="{91DE4E1A-6DA9-5D41-9DB5-21149FC9505F}" name="sample name"/>
     <tableColumn id="7" xr3:uid="{E7F73DE6-44A2-FD49-95BC-9E263FB79FB0}" name="barcode"/>
-    <tableColumn id="2" xr3:uid="{D3E7E880-2BC6-B94A-AFA4-408237577810}" name="DNA size" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D3E7E880-2BC6-B94A-AFA4-408237577810}" name="DNA size" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{AF07D2D6-012E-8643-901A-5055CCEAF026}" name="ng/ul"/>
-    <tableColumn id="4" xr3:uid="{80D148B5-CECA-CA44-B1DD-F9E1A8DAA6A0}" name="fmol/rxn" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{80D148B5-CECA-CA44-B1DD-F9E1A8DAA6A0}" name="fmol/rxn" dataDxfId="4">
       <calculatedColumnFormula array="1">_xlfn.IFS(ISBLANK(Table1[[#This Row],[DNA size]]), 0, TRUE, F9/((E9*617.96)+36.04) * 1000000*Table1[[#This Row],[ul DNA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6A4DD60B-B1AB-FF44-9E4F-4697D7C0CC9E}" name="ul DNA" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{6A4DD60B-B1AB-FF44-9E4F-4697D7C0CC9E}" name="ul DNA" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.IFS(ISBLANK(Table1[[#This Row],[source well]]), 0, $J$5/Table1[[#This Row],[ng/ul]] &gt; 10, 10, $J$5/Table1[[#This Row],[ng/ul]] &lt; 0.5, 0.5, TRUE, $J$5/Table1[[#This Row],[ng/ul]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{53D08A06-9EBD-1143-A0BC-3E9BC0C89175}" name="ul water to 10" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{53D08A06-9EBD-1143-A0BC-3E9BC0C89175}" name="ul water to 10" dataDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[ul DNA]]=0,0,10-Table1[[#This Row],[ul DNA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0EE7AD1A-A1CC-364C-B346-C43B6AB6BFEF}" name="dest well" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{DDAE90F6-C57C-A64E-B7AF-286C3EB0FE38}" name="barcode well" dataDxfId="4">
+    <tableColumn id="10" xr3:uid="{0EE7AD1A-A1CC-364C-B346-C43B6AB6BFEF}" name="dest well" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{DDAE90F6-C57C-A64E-B7AF-286C3EB0FE38}" name="barcode well" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1702,7 +1701,7 @@
   <dimension ref="B1:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1745,7 +1744,7 @@
       <c r="I4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="17"/>
+      <c r="J4" s="16"/>
       <c r="M4" s="1" t="s">
         <v>311</v>
       </c>
@@ -1758,21 +1757,21 @@
         <v>329</v>
       </c>
       <c r="J5" s="8">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="17"/>
       <c r="I6" t="s">
         <v>332</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="20" t="s">
         <v>312</v>
       </c>
       <c r="N6" s="11" t="s">
@@ -1786,8 +1785,8 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="G7" s="19"/>
-      <c r="M7" s="21" t="s">
+      <c r="G7" s="18"/>
+      <c r="M7" s="20" t="s">
         <v>314</v>
       </c>
       <c r="N7" s="11">
@@ -1831,7 +1830,7 @@
       <c r="K8" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="20" t="s">
         <v>309</v>
       </c>
       <c r="N8" s="11" t="s">
@@ -1862,15 +1861,15 @@
       </c>
       <c r="G9" s="14" cm="1">
         <f t="array" ref="G9">_xlfn.IFS(ISBLANK(Table1[[#This Row],[DNA size]]), 0, TRUE, F9/((E9*617.96)+36.04) * 1000000*Table1[[#This Row],[ul DNA]])</f>
-        <v>5.3940819037525722</v>
+        <v>2.6970409518762861</v>
       </c>
       <c r="H9" s="2" cm="1">
         <f t="array" ref="H9">_xlfn.IFS(ISBLANK(Table1[[#This Row],[source well]]), 0, $J$5/Table1[[#This Row],[ng/ul]] &gt; 10, 10, $J$5/Table1[[#This Row],[ng/ul]] &lt; 0.5, 0.5, TRUE, $J$5/Table1[[#This Row],[ng/ul]])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2">
         <f>IF(Table1[[#This Row],[ul DNA]]=0,0,10-Table1[[#This Row],[ul DNA]])</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>105</v>
@@ -1879,7 +1878,7 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
         <v>A01</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="20" t="s">
         <v>319</v>
       </c>
       <c r="N9" s="11" t="s">
@@ -1904,15 +1903,15 @@
       </c>
       <c r="G10" s="14" cm="1">
         <f t="array" ref="G10">_xlfn.IFS(ISBLANK(Table1[[#This Row],[DNA size]]), 0, TRUE, F10/((E10*617.96)+36.04) * 1000000*Table1[[#This Row],[ul DNA]])</f>
-        <v>5.3940819037525722</v>
+        <v>2.6970409518762861</v>
       </c>
       <c r="H10" s="2" cm="1">
         <f t="array" ref="H10">_xlfn.IFS(ISBLANK(Table1[[#This Row],[source well]]), 0, $J$5/Table1[[#This Row],[ng/ul]] &gt; 10, 10, $J$5/Table1[[#This Row],[ng/ul]] &lt; 0.5, 0.5, TRUE, $J$5/Table1[[#This Row],[ng/ul]])</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I10" s="2">
         <f>IF(Table1[[#This Row],[ul DNA]]=0,0,10-Table1[[#This Row],[ul DNA]])</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>106</v>
@@ -1921,7 +1920,7 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
         <v>B01</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="20" t="s">
         <v>318</v>
       </c>
       <c r="N10" s="11" t="s">
@@ -1946,15 +1945,15 @@
       </c>
       <c r="G11" s="14" cm="1">
         <f t="array" ref="G11">_xlfn.IFS(ISBLANK(Table1[[#This Row],[DNA size]]), 0, TRUE, F11/((E11*617.96)+36.04) * 1000000*Table1[[#This Row],[ul DNA]])</f>
-        <v>5.3940819037525722</v>
+        <v>2.6970409518762861</v>
       </c>
       <c r="H11" s="2" cm="1">
         <f t="array" ref="H11">_xlfn.IFS(ISBLANK(Table1[[#This Row],[source well]]), 0, $J$5/Table1[[#This Row],[ng/ul]] &gt; 10, 10, $J$5/Table1[[#This Row],[ng/ul]] &lt; 0.5, 0.5, TRUE, $J$5/Table1[[#This Row],[ng/ul]])</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="2">
         <f>IF(Table1[[#This Row],[ul DNA]]=0,0,10-Table1[[#This Row],[ul DNA]])</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>107</v>
@@ -1996,7 +1995,7 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
         <v>D01</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="20" t="s">
         <v>322</v>
       </c>
       <c r="N12" s="11" t="s">
@@ -2024,12 +2023,12 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
         <v/>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="20" t="s">
         <v>336</v>
       </c>
       <c r="N13">
         <f>COUNTA(Table1[source well])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.2">
@@ -2053,12 +2052,12 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
         <v/>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="M14" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <f>N13*11</f>
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
@@ -2082,12 +2081,12 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
         <v/>
       </c>
-      <c r="M15" s="21" t="s">
+      <c r="M15" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="21">
         <f>SUM(Table1[fmol/rxn])</f>
-        <v>21.576327615010289</v>
+        <v>21.576296156408109</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
@@ -2113,25 +2112,39 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E17" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
       <c r="G17" s="14" cm="1">
         <f t="array" ref="G17">_xlfn.IFS(ISBLANK(Table1[[#This Row],[DNA size]]), 0, TRUE, F17/((E17*617.96)+36.04) * 1000000*Table1[[#This Row],[ul DNA]])</f>
-        <v>0</v>
+        <v>8.0910913970266769</v>
       </c>
       <c r="H17" s="2" cm="1">
         <f t="array" ref="H17">_xlfn.IFS(ISBLANK(Table1[[#This Row],[source well]]), 0, $J$5/Table1[[#This Row],[ng/ul]] &gt; 10, 10, $J$5/Table1[[#This Row],[ng/ul]] &lt; 0.5, 0.5, TRUE, $J$5/Table1[[#This Row],[ng/ul]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2">
         <f>IF(Table1[[#This Row],[ul DNA]]=0,0,10-Table1[[#This Row],[ul DNA]])</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>113</v>
       </c>
       <c r="K17" s="9" t="str">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[barcode]],Table2[name],Table2[well],"")</f>
-        <v/>
+        <v>D01</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -5472,7 +5485,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5527,7 +5540,7 @@
       </c>
       <c r="C2" s="9">
         <f>main!H9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>IF(C2=0, "", "A01")</f>
@@ -5538,7 +5551,7 @@
       </c>
       <c r="F2" s="9">
         <f>main!I9</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D9,Table2[name],Table2[well],"")</f>
@@ -5562,7 +5575,7 @@
       </c>
       <c r="C3" s="9">
         <f>main!H10</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8" t="str">
         <f t="shared" ref="D3:D66" si="0">IF(C3=0, "", "A01")</f>
@@ -5573,7 +5586,7 @@
       </c>
       <c r="F3" s="9">
         <f>main!I10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D10,Table2[name],Table2[well],"")</f>
@@ -5597,7 +5610,7 @@
       </c>
       <c r="C4" s="9">
         <f>main!H11</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5608,7 +5621,7 @@
       </c>
       <c r="F4" s="9">
         <f>main!I11</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G4" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D11,Table2[name],Table2[well],"")</f>
@@ -5800,36 +5813,36 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="str">
         <f>TEXT(main!B17, "")</f>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C10" s="9">
         <f>main!H17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>A01</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>113</v>
       </c>
       <c r="F10" s="9">
         <f>main!I17</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G10" s="8" t="str">
         <f>_xlfn.XLOOKUP(main!D17,Table2[name],Table2[well],"")</f>
-        <v/>
+        <v>D01</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>